<commit_message>
Update Group 1 Team CBA - MITR.xlsx
</commit_message>
<xml_diff>
--- a/Project Documents/Group 1 Team CBA - MITR.xlsx
+++ b/Project Documents/Group 1 Team CBA - MITR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael Chung\MITRE\MITR-RCC-Project\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA919E0E-F0BD-435A-AA5C-881907FF4470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FAA9A9-21E4-499C-9FB4-B80151D3172E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1128,8 +1128,8 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G46" zoomScale="103" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="103" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1472,9 +1472,7 @@
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="6">
-        <v>100</v>
-      </c>
+      <c r="B15" s="6"/>
       <c r="C15" s="6">
         <v>0</v>
       </c>
@@ -1489,7 +1487,7 @@
       </c>
       <c r="G15" s="6">
         <f t="shared" si="4"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="2"/>
@@ -1583,7 +1581,7 @@
       </c>
       <c r="B19" s="3">
         <f t="shared" ref="B19:F19" si="5">SUM(B14:B18)</f>
-        <v>1052</v>
+        <v>952</v>
       </c>
       <c r="C19" s="3">
         <f t="shared" si="5"/>
@@ -1603,7 +1601,7 @@
       </c>
       <c r="G19" s="6">
         <f t="shared" si="4"/>
-        <v>4713</v>
+        <v>4613</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="2"/>
@@ -1615,7 +1613,7 @@
       </c>
       <c r="B20" s="6">
         <f>B12-B19</f>
-        <v>-1052</v>
+        <v>-952</v>
       </c>
       <c r="C20" s="6">
         <f>C12-C19</f>
@@ -1644,23 +1642,23 @@
       </c>
       <c r="B21" s="3">
         <f>B20</f>
-        <v>-1052</v>
+        <v>-952</v>
       </c>
       <c r="C21" s="3">
         <f t="shared" ref="C21:F21" si="6">B21+C20</f>
-        <v>-1526</v>
+        <v>-1426</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" si="6"/>
-        <v>-1100</v>
+        <v>-1000</v>
       </c>
       <c r="E21" s="6">
         <f t="shared" si="6"/>
-        <v>476</v>
+        <v>576</v>
       </c>
       <c r="F21" s="6">
         <f t="shared" si="6"/>
-        <v>3027</v>
+        <v>3127</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="4"/>
@@ -1688,11 +1686,11 @@
       </c>
       <c r="B23" s="14">
         <f>NPV(A23,C20:F20)+B20</f>
-        <v>1795.5964756505696</v>
+        <v>1895.5964756505696</v>
       </c>
       <c r="C23" s="11">
         <f>IRR(B20:F20)</f>
-        <v>0.4211043734524893</v>
+        <v>0.45660844349767116</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1708,11 +1706,11 @@
       </c>
       <c r="B24" s="4">
         <f>NPV(A24,C20:F20)+B20</f>
-        <v>239.211554998579</v>
+        <v>339.211554998579</v>
       </c>
       <c r="C24" s="11">
         <f>IRR(B20:F20)</f>
-        <v>0.4211043734524893</v>
+        <v>0.45660844349767116</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2398,7 +2396,7 @@
         <v>200</v>
       </c>
       <c r="N52" s="18">
-        <f>ROUNDDOWN(M52/$M$61,2)</f>
+        <f t="shared" ref="N52:N59" si="10">ROUNDDOWN(M52/$M$61,2)</f>
         <v>0.08</v>
       </c>
       <c r="O52" s="19">
@@ -2434,7 +2432,7 @@
         <v>400</v>
       </c>
       <c r="N53" s="18">
-        <f>ROUNDDOWN(M53/$M$61,2)</f>
+        <f t="shared" si="10"/>
         <v>0.16</v>
       </c>
       <c r="O53" s="19">
@@ -2470,7 +2468,7 @@
         <v>500</v>
       </c>
       <c r="N54" s="18">
-        <f>ROUNDDOWN(M54/$M$61,2)</f>
+        <f t="shared" si="10"/>
         <v>0.2</v>
       </c>
       <c r="O54" s="19">
@@ -2506,7 +2504,7 @@
         <v>300</v>
       </c>
       <c r="N55" s="18">
-        <f>ROUNDDOWN(M55/$M$61,2)</f>
+        <f t="shared" si="10"/>
         <v>0.12</v>
       </c>
       <c r="O55" s="19">
@@ -2542,7 +2540,7 @@
         <v>200</v>
       </c>
       <c r="N56" s="18">
-        <f>ROUNDDOWN(M56/$M$61,2)</f>
+        <f t="shared" si="10"/>
         <v>0.08</v>
       </c>
       <c r="O56" s="19">
@@ -2578,7 +2576,7 @@
         <v>300</v>
       </c>
       <c r="N57" s="18">
-        <f>ROUNDDOWN(M57/$M$61,2)</f>
+        <f t="shared" si="10"/>
         <v>0.12</v>
       </c>
       <c r="O57" s="19">
@@ -2614,7 +2612,7 @@
         <v>100</v>
       </c>
       <c r="N58" s="18">
-        <f>ROUNDDOWN(M58/$M$61,2)</f>
+        <f t="shared" si="10"/>
         <v>0.04</v>
       </c>
       <c r="O58" s="19">
@@ -2650,7 +2648,7 @@
         <v>300</v>
       </c>
       <c r="N59" s="18">
-        <f>ROUNDDOWN(M59/$M$61,2)</f>
+        <f t="shared" si="10"/>
         <v>0.12</v>
       </c>
       <c r="O59" s="19">
@@ -2711,14 +2709,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9392a558-f998-4c52-9879-76813e889e56" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2727,7 +2717,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003464484D0C360A40AF77D5C66939F595" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aed76de4be4a95df9a7b631dcf6d49df">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9392a558-f998-4c52-9879-76813e889e56" xmlns:ns4="637bf4fa-d8b4-4807-8184-b158808b27be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bd00252ac23e977623ead2ac626c119" ns3:_="" ns4:_="">
     <xsd:import namespace="9392a558-f998-4c52-9879-76813e889e56"/>
@@ -2910,24 +2900,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD634264-3B53-4770-BDFB-3CA228F6032C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="9392a558-f998-4c52-9879-76813e889e56"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="637bf4fa-d8b4-4807-8184-b158808b27be"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9392a558-f998-4c52-9879-76813e889e56" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA92F263-4EA8-4BDD-8F77-C9F81D9D771D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2935,7 +2916,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5223E04-D98F-4340-A226-39655CF2A234}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2952,4 +2933,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD634264-3B53-4770-BDFB-3CA228F6032C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="9392a558-f998-4c52-9879-76813e889e56"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="637bf4fa-d8b4-4807-8184-b158808b27be"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>